<commit_message>
Responded to some comments
</commit_message>
<xml_diff>
--- a/Intervention 1/Scenario Analysis Enterobacteriaceae.xlsx
+++ b/Intervention 1/Scenario Analysis Enterobacteriaceae.xlsx
@@ -94,10 +94,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>-4.74411587922855E9</v>
+        <v>-4.73617866047286E9</v>
       </c>
       <c r="C2" t="n">
-        <v>-4.745140991881192E9</v>
+        <v>-4.743118513867647E9</v>
       </c>
     </row>
     <row r="3">
@@ -105,10 +105,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>-4.742248671192513E9</v>
+        <v>-4.72637420022957E9</v>
       </c>
       <c r="C3" t="n">
-        <v>-4.744298899186662E9</v>
+        <v>-4.740253936489744E9</v>
       </c>
     </row>
     <row r="4">
@@ -116,10 +116,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>-4.738514242196011E9</v>
+        <v>-4.706765166463247E9</v>
       </c>
       <c r="C4" t="n">
-        <v>-4.742614708939799E9</v>
+        <v>-4.734524756866552E9</v>
       </c>
     </row>
     <row r="5">
@@ -127,10 +127,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>-4.734032904653097E9</v>
+        <v>-4.683234126569675E9</v>
       </c>
       <c r="C5" t="n">
-        <v>-4.740593672093796E9</v>
+        <v>-4.727649697551818E9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>